<commit_message>
Ablation study supplementary figure
</commit_message>
<xml_diff>
--- a/data/TaxVAMB_Source_Data.xlsx
+++ b/data/TaxVAMB_Source_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmb127/Documents/TaxVAMB_paper_figures/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B18EF8-2413-F348-8ECB-BC4F222F2176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E857A93-C72A-D84A-8C1F-08A718BC6B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1680" yWindow="-23500" windowWidth="38400" windowHeight="23500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,14 +21,15 @@
     <sheet name="Figure 5c" sheetId="6" r:id="rId6"/>
     <sheet name="Figure 6b" sheetId="7" r:id="rId7"/>
     <sheet name="Figure 6c" sheetId="8" r:id="rId8"/>
-    <sheet name="Supplementary Figure 3" sheetId="14" r:id="rId9"/>
-    <sheet name="Supplementary Figure 4" sheetId="9" r:id="rId10"/>
-    <sheet name="Supplementary Figure 5" sheetId="10" r:id="rId11"/>
-    <sheet name="Supplementary Figure 6" sheetId="11" r:id="rId12"/>
-    <sheet name="Supplementary Figure 7b" sheetId="12" r:id="rId13"/>
-    <sheet name="Supplementary Figure 8" sheetId="13" r:id="rId14"/>
+    <sheet name="Supplementary Figure" sheetId="15" r:id="rId9"/>
+    <sheet name="Supplementary Figure 3" sheetId="14" r:id="rId10"/>
+    <sheet name="Supplementary Figure 4" sheetId="9" r:id="rId11"/>
+    <sheet name="Supplementary Figure 5" sheetId="10" r:id="rId12"/>
+    <sheet name="Supplementary Figure 6" sheetId="11" r:id="rId13"/>
+    <sheet name="Supplementary Figure 7b" sheetId="12" r:id="rId14"/>
+    <sheet name="Supplementary Figure 8" sheetId="13" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="241">
   <si>
     <t>Dataset</t>
   </si>
@@ -739,6 +740,36 @@
   </si>
   <si>
     <t>gtdbtk</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Genomes</t>
+  </si>
+  <si>
+    <t>Assemblies</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>vamb</t>
+  </si>
+  <si>
+    <t>taxvamb</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Taxometer</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -748,7 +779,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -798,6 +829,26 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -970,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1030,6 +1081,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4282,6 +4342,1025 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13ED3BFC-EC67-0148-8780-6B694AAD2802}">
+  <dimension ref="A1:C91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="10">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="10">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="14">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="6">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="10">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="6">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="6">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="10">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="6">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="6">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="6">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="6">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="14">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="6">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="6">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="6">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="14">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="6">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="6">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="14">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="6">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="6">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="6">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="10">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="6">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="6">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="6">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="6">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" s="14">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" s="6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" s="6">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" s="6">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" s="14">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="6">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" s="6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" s="14">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="6">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" s="6">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" s="6">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C87" s="14">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" s="6">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" s="6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C90" s="6">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="6">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5303,7 +6382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5476,7 +6555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6561,7 +7640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10517,7 +11596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -14480,7 +15559,9 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -18445,1017 +19526,458 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13ED3BFC-EC67-0148-8780-6B694AAD2802}">
-  <dimension ref="A1:C91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD97C-3359-9C47-AB14-B0091E523971}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="31">
+        <v>92</v>
+      </c>
+      <c r="D2" s="31">
+        <v>166</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="31">
+        <v>98</v>
+      </c>
+      <c r="D3" s="31">
+        <v>116</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="31">
+        <v>112</v>
+      </c>
+      <c r="D4" s="31">
+        <v>186</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="31">
+        <v>141</v>
+      </c>
+      <c r="D5" s="31">
+        <v>206</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="31">
+        <v>148</v>
+      </c>
+      <c r="D6" s="31">
+        <v>179</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="31">
+        <v>102</v>
+      </c>
+      <c r="D7" s="31">
+        <v>169</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="31">
+        <v>121</v>
+      </c>
+      <c r="D8" s="31">
+        <v>140</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="31">
+        <v>121</v>
+      </c>
+      <c r="D9" s="31">
+        <v>135</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="31">
+        <v>135</v>
+      </c>
+      <c r="D10" s="31">
+        <v>156</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="31">
+        <v>97</v>
+      </c>
+      <c r="D11" s="31">
+        <v>124</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="31">
+        <v>77</v>
+      </c>
+      <c r="D12" s="31">
+        <v>100</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="31">
+        <v>105</v>
+      </c>
+      <c r="D13" s="31">
+        <v>113</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="B14" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="31">
+        <v>76</v>
+      </c>
+      <c r="D14" s="31">
+        <v>122</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="31">
+        <v>68</v>
+      </c>
+      <c r="D15" s="31">
+        <v>162</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="31">
+        <v>90</v>
+      </c>
+      <c r="D16" s="31">
+        <v>193</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15">
+      <c r="A17" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="31">
+        <v>82</v>
+      </c>
+      <c r="D17" s="31">
+        <v>161</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="31">
+        <v>125</v>
+      </c>
+      <c r="D18" s="31">
+        <v>148</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15">
+      <c r="A19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="31">
+        <v>138</v>
+      </c>
+      <c r="D19" s="31">
+        <v>187</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15">
+      <c r="A20" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="31">
+        <v>105</v>
+      </c>
+      <c r="D20" s="31">
+        <v>155</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15">
+      <c r="A21" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B21" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="31">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="D21" s="31">
+        <v>124</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15">
+      <c r="A22" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="31">
+        <v>41</v>
+      </c>
+      <c r="D22" s="31">
+        <v>87</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15">
+      <c r="A23" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="B23" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="31">
+        <v>105</v>
+      </c>
+      <c r="D23" s="31">
+        <v>115</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="A24" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="31">
+        <v>65</v>
+      </c>
+      <c r="D24" s="31">
+        <v>95</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15">
+      <c r="A25" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="10">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="B25" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="31">
+        <v>62</v>
+      </c>
+      <c r="D25" s="31">
+        <v>88</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15">
+      <c r="A26" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="6">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="6">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="14">
+      <c r="B26" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="31">
+        <v>58</v>
+      </c>
+      <c r="D26" s="31">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="6">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="14">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="6">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="6">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="10">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="6">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="6">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="6">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="6">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="14">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="6">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="6">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="6">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="10">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="14">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="6">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="6">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="6">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="10">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="6">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="6">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="6">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="6">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="6">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" s="14">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="6">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="6">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="6">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="10">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="6">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="6">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="6">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="6">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="6">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" s="14">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C53" s="6">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="6">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="6">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C56" s="6">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="14">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="6">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="6">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C60" s="6">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="6">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="14">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="6">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="6">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" s="6">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="10">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="6">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="6">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="6">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="6">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="6">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" s="14">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C73" s="6">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74" s="6">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C75" s="6">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C76" s="6">
+      <c r="E26" s="35" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C77" s="14">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="6">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C79" s="6">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" s="6">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C81" s="6">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C82" s="14">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C83" s="6">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C84" s="6">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C85" s="6">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C86" s="6">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C87" s="14">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C88" s="6">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C89" s="6">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C90" s="6">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C91" s="6">
-        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supplementary Figure with MMSeqs databases
</commit_message>
<xml_diff>
--- a/data/TaxVAMB_Source_Data.xlsx
+++ b/data/TaxVAMB_Source_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmb127/Documents/TaxVAMB_paper_figures/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E857A93-C72A-D84A-8C1F-08A718BC6B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5076F120-9E65-E94F-B879-6B8FA7FFDDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1680" yWindow="-23500" windowWidth="38400" windowHeight="23500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,13 +21,14 @@
     <sheet name="Figure 5c" sheetId="6" r:id="rId6"/>
     <sheet name="Figure 6b" sheetId="7" r:id="rId7"/>
     <sheet name="Figure 6c" sheetId="8" r:id="rId8"/>
-    <sheet name="Supplementary Figure" sheetId="15" r:id="rId9"/>
-    <sheet name="Supplementary Figure 3" sheetId="14" r:id="rId10"/>
-    <sheet name="Supplementary Figure 4" sheetId="9" r:id="rId11"/>
-    <sheet name="Supplementary Figure 5" sheetId="10" r:id="rId12"/>
-    <sheet name="Supplementary Figure 6" sheetId="11" r:id="rId13"/>
-    <sheet name="Supplementary Figure 7b" sheetId="12" r:id="rId14"/>
-    <sheet name="Supplementary Figure 8" sheetId="13" r:id="rId15"/>
+    <sheet name="Supplementary Figure Databases" sheetId="16" r:id="rId9"/>
+    <sheet name="Supplementary Figure" sheetId="15" r:id="rId10"/>
+    <sheet name="Supplementary Figure 3" sheetId="14" r:id="rId11"/>
+    <sheet name="Supplementary Figure 4" sheetId="9" r:id="rId12"/>
+    <sheet name="Supplementary Figure 5" sheetId="10" r:id="rId13"/>
+    <sheet name="Supplementary Figure 6" sheetId="11" r:id="rId14"/>
+    <sheet name="Supplementary Figure 7b" sheetId="12" r:id="rId15"/>
+    <sheet name="Supplementary Figure 8" sheetId="13" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="257">
   <si>
     <t>Dataset</t>
   </si>
@@ -770,6 +771,54 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>HQ_bins</t>
+  </si>
+  <si>
+    <t>MQ_bins</t>
+  </si>
+  <si>
+    <t>vamb_is_with_reclustering</t>
+  </si>
+  <si>
+    <t>no_predictor</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>vamb_based_tool</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>bee_metagenome_PRJNA1007366</t>
+  </si>
+  <si>
+    <t>kalmari_taxvamb_default</t>
+  </si>
+  <si>
+    <t>human_saliva_oral_PRJDB16210</t>
+  </si>
+  <si>
+    <t>PRJNA1003562</t>
+  </si>
+  <si>
+    <t>PRJNA638805</t>
+  </si>
+  <si>
+    <t>PRJNA783873</t>
+  </si>
+  <si>
+    <t>vag_infert_PRJNA1078345</t>
+  </si>
+  <si>
+    <t>trembl_taxvamb_default</t>
+  </si>
+  <si>
+    <t>run_taxvamb_gtdb_w_unknown</t>
   </si>
 </sst>
 </file>
@@ -779,7 +828,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -849,6 +898,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1081,15 +1138,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4342,6 +4401,466 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD97C-3359-9C47-AB14-B0091E523971}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="31">
+        <v>92</v>
+      </c>
+      <c r="D2" s="31">
+        <v>166</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="31">
+        <v>98</v>
+      </c>
+      <c r="D3" s="31">
+        <v>116</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="31">
+        <v>112</v>
+      </c>
+      <c r="D4" s="31">
+        <v>186</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="31">
+        <v>141</v>
+      </c>
+      <c r="D5" s="31">
+        <v>206</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="31">
+        <v>148</v>
+      </c>
+      <c r="D6" s="31">
+        <v>179</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="31">
+        <v>102</v>
+      </c>
+      <c r="D7" s="31">
+        <v>169</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="31">
+        <v>121</v>
+      </c>
+      <c r="D8" s="31">
+        <v>140</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="31">
+        <v>121</v>
+      </c>
+      <c r="D9" s="31">
+        <v>135</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C10" s="31">
+        <v>135</v>
+      </c>
+      <c r="D10" s="31">
+        <v>156</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="31">
+        <v>97</v>
+      </c>
+      <c r="D11" s="31">
+        <v>124</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="31">
+        <v>77</v>
+      </c>
+      <c r="D12" s="31">
+        <v>100</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="31">
+        <v>105</v>
+      </c>
+      <c r="D13" s="31">
+        <v>113</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="31">
+        <v>76</v>
+      </c>
+      <c r="D14" s="31">
+        <v>122</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="31">
+        <v>68</v>
+      </c>
+      <c r="D15" s="31">
+        <v>162</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="31">
+        <v>90</v>
+      </c>
+      <c r="D16" s="31">
+        <v>193</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15">
+      <c r="A17" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="31">
+        <v>82</v>
+      </c>
+      <c r="D17" s="31">
+        <v>161</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="31">
+        <v>125</v>
+      </c>
+      <c r="D18" s="31">
+        <v>148</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15">
+      <c r="A19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="31">
+        <v>138</v>
+      </c>
+      <c r="D19" s="31">
+        <v>187</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15">
+      <c r="A20" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="31">
+        <v>105</v>
+      </c>
+      <c r="D20" s="31">
+        <v>155</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="31">
+        <v>103</v>
+      </c>
+      <c r="D21" s="31">
+        <v>124</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15">
+      <c r="A22" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="31">
+        <v>41</v>
+      </c>
+      <c r="D22" s="31">
+        <v>87</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="31">
+        <v>105</v>
+      </c>
+      <c r="D23" s="31">
+        <v>115</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="A24" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="31">
+        <v>65</v>
+      </c>
+      <c r="D24" s="31">
+        <v>95</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15">
+      <c r="A25" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="31">
+        <v>62</v>
+      </c>
+      <c r="D25" s="31">
+        <v>88</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15">
+      <c r="A26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="31">
+        <v>58</v>
+      </c>
+      <c r="D26" s="31">
+        <v>68</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13ED3BFC-EC67-0148-8780-6B694AAD2802}">
   <dimension ref="A1:C91"/>
   <sheetViews>
@@ -5360,7 +5879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6382,7 +6901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6555,7 +7074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7640,7 +8159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -11596,7 +12115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -19526,459 +20045,511 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BCD97C-3359-9C47-AB14-B0091E523971}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850E37AB-6A76-774E-889D-1138ECDECC2C}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="31" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="34">
+        <v>6</v>
+      </c>
+      <c r="B2" s="34">
+        <v>10</v>
+      </c>
+      <c r="C2" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="34">
+        <v>71</v>
+      </c>
+      <c r="B3" s="34">
+        <v>266</v>
+      </c>
+      <c r="C3" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="34">
+        <v>26</v>
+      </c>
+      <c r="B4" s="34">
+        <v>64</v>
+      </c>
+      <c r="C4" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="34">
+        <v>116</v>
+      </c>
+      <c r="B5" s="34">
+        <v>446</v>
+      </c>
+      <c r="C5" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="F5" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="34">
+        <v>33</v>
+      </c>
+      <c r="B6" s="34">
+        <v>178</v>
+      </c>
+      <c r="C6" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="34">
+        <v>5</v>
+      </c>
+      <c r="B7" s="34">
+        <v>11</v>
+      </c>
+      <c r="C7" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="34">
+        <v>5</v>
+      </c>
+      <c r="B8" s="34">
+        <v>10</v>
+      </c>
+      <c r="C8" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="34">
+        <v>120</v>
+      </c>
+      <c r="B9" s="34">
+        <v>338</v>
+      </c>
+      <c r="C9" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F9" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="34">
+        <v>25</v>
+      </c>
+      <c r="B10" s="34">
+        <v>77</v>
+      </c>
+      <c r="C10" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="34">
+        <v>148</v>
+      </c>
+      <c r="B11" s="34">
+        <v>415</v>
+      </c>
+      <c r="C11" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="34">
+        <v>41</v>
+      </c>
+      <c r="B12" s="34">
+        <v>259</v>
+      </c>
+      <c r="C12" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F12" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="34">
+        <v>7</v>
+      </c>
+      <c r="B13" s="34">
         <v>12</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2" s="31">
-        <v>92</v>
-      </c>
-      <c r="D2" s="31">
-        <v>166</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="31" t="s">
+      <c r="C13" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="F13" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="34">
+        <v>4</v>
+      </c>
+      <c r="B14" s="34">
         <v>12</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="31">
-        <v>98</v>
-      </c>
-      <c r="D3" s="31">
-        <v>116</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="31" t="s">
+      <c r="C14" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="F14" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="34">
+        <v>201</v>
+      </c>
+      <c r="B15" s="34">
+        <v>515</v>
+      </c>
+      <c r="C15" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="F15" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="34">
+        <v>40</v>
+      </c>
+      <c r="B16" s="34">
+        <v>317</v>
+      </c>
+      <c r="C16" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F16" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="34">
+        <v>132</v>
+      </c>
+      <c r="B17" s="34">
+        <v>355</v>
+      </c>
+      <c r="C17" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="34">
+        <v>26</v>
+      </c>
+      <c r="B18" s="34">
+        <v>90</v>
+      </c>
+      <c r="C18" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="F18" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="34">
+        <v>7</v>
+      </c>
+      <c r="B19" s="34">
         <v>12</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="31">
-        <v>112</v>
-      </c>
-      <c r="D4" s="31">
-        <v>186</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" s="31">
-        <v>141</v>
-      </c>
-      <c r="D5" s="31">
-        <v>206</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C6" s="31">
-        <v>148</v>
-      </c>
-      <c r="D6" s="31">
-        <v>179</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C7" s="31">
-        <v>102</v>
-      </c>
-      <c r="D7" s="31">
-        <v>169</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C8" s="31">
-        <v>121</v>
-      </c>
-      <c r="D8" s="31">
-        <v>140</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" s="31">
-        <v>121</v>
-      </c>
-      <c r="D9" s="31">
-        <v>135</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C10" s="31">
-        <v>135</v>
-      </c>
-      <c r="D10" s="31">
-        <v>156</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C11" s="31">
-        <v>97</v>
-      </c>
-      <c r="D11" s="31">
-        <v>124</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C12" s="31">
-        <v>77</v>
-      </c>
-      <c r="D12" s="31">
-        <v>100</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="A13" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" s="31">
-        <v>105</v>
-      </c>
-      <c r="D13" s="31">
-        <v>113</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C14" s="31">
-        <v>76</v>
-      </c>
-      <c r="D14" s="31">
-        <v>122</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C15" s="31">
-        <v>68</v>
-      </c>
-      <c r="D15" s="31">
-        <v>162</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C16" s="31">
-        <v>90</v>
-      </c>
-      <c r="D16" s="31">
-        <v>193</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15">
-      <c r="A17" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C17" s="31">
-        <v>82</v>
-      </c>
-      <c r="D17" s="31">
-        <v>161</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15">
-      <c r="A18" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C18" s="31">
-        <v>125</v>
-      </c>
-      <c r="D18" s="31">
-        <v>148</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15">
-      <c r="A19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" s="31">
-        <v>138</v>
-      </c>
-      <c r="D19" s="31">
-        <v>187</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C20" s="31">
-        <v>105</v>
-      </c>
-      <c r="D20" s="31">
-        <v>155</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15">
-      <c r="A21" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="C21" s="31">
-        <v>103</v>
-      </c>
-      <c r="D21" s="31">
-        <v>124</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15">
-      <c r="A22" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C22" s="31">
-        <v>41</v>
-      </c>
-      <c r="D22" s="31">
-        <v>87</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15">
-      <c r="A23" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C23" s="31">
-        <v>105</v>
-      </c>
-      <c r="D23" s="31">
-        <v>115</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15">
-      <c r="A24" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C24" s="31">
-        <v>65</v>
-      </c>
-      <c r="D24" s="31">
-        <v>95</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15">
-      <c r="A25" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C25" s="31">
-        <v>62</v>
-      </c>
-      <c r="D25" s="31">
-        <v>88</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15">
-      <c r="A26" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="C26" s="31">
-        <v>58</v>
-      </c>
-      <c r="D26" s="31">
-        <v>68</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>237</v>
-      </c>
+      <c r="C19" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F19" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Semibin without reclustering rerun
</commit_message>
<xml_diff>
--- a/data/TaxVAMB_Source_Data.xlsx
+++ b/data/TaxVAMB_Source_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmb127/Documents/TaxVAMB_paper_figures/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411FD774-34E1-3D48-AC20-1F31B2255DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7181DA10-C4DA-BD40-9E40-D01945731EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8400" yWindow="-28200" windowWidth="51200" windowHeight="28200" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8400" yWindow="-28200" windowWidth="51200" windowHeight="28200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 2a" sheetId="19" r:id="rId1"/>
@@ -2203,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E3FEE1-33E1-CA46-9B36-FA8A8BC0E01C}">
   <dimension ref="A1:I341"/>
   <sheetViews>
-    <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="G347" sqref="G347"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="G350" sqref="G350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9980,7 +9980,7 @@
         <v>92</v>
       </c>
       <c r="I259" t="str">
-        <f t="shared" ref="I259:I281" si="4">_xlfn.CONCAT(G259,"_",D259)</f>
+        <f t="shared" ref="I259:I271" si="4">_xlfn.CONCAT(G259,"_",D259)</f>
         <v>kalmari_taxvamb_default_FALSE</v>
       </c>
     </row>
@@ -10364,14 +10364,14 @@
         <v>0</v>
       </c>
       <c r="G272" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H272" s="22">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="I272" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" ref="I272:I303" si="5">_xlfn.CONCAT(G272,"_",D272)</f>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="273" spans="1:9">
@@ -10394,14 +10394,14 @@
         <v>0</v>
       </c>
       <c r="G273" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H273" s="22">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="I273" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="274" spans="1:9">
@@ -10424,14 +10424,14 @@
         <v>0</v>
       </c>
       <c r="G274" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H274" s="22">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="I274" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="275" spans="1:9">
@@ -10454,14 +10454,14 @@
         <v>0</v>
       </c>
       <c r="G275" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H275" s="22">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="I275" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="276" spans="1:9">
@@ -10484,14 +10484,14 @@
         <v>0</v>
       </c>
       <c r="G276" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H276" s="22">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="I276" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="277" spans="1:9">
@@ -10514,14 +10514,14 @@
         <v>0</v>
       </c>
       <c r="G277" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H277" s="22">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="I277" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -10544,14 +10544,14 @@
         <v>0</v>
       </c>
       <c r="G278" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H278" s="22">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="I278" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="279" spans="1:9">
@@ -10574,14 +10574,14 @@
         <v>0</v>
       </c>
       <c r="G279" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H279" s="22">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="I279" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="280" spans="1:9">
@@ -10604,14 +10604,14 @@
         <v>0</v>
       </c>
       <c r="G280" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H280" s="22">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="I280" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="281" spans="1:9">
@@ -10634,14 +10634,14 @@
         <v>0</v>
       </c>
       <c r="G281" s="22" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H281" s="22">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="I281" t="str">
-        <f t="shared" si="4"/>
-        <v>semibin_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>metadecoder_FALSE</v>
       </c>
     </row>
     <row r="282" spans="1:9">
@@ -10661,17 +10661,17 @@
         <v>0</v>
       </c>
       <c r="F282" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G282" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H282" s="22">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I282" t="str">
-        <f>_xlfn.CONCAT(G282,"_",D282)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="283" spans="1:9">
@@ -10691,17 +10691,17 @@
         <v>0</v>
       </c>
       <c r="F283" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G283" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H283" s="22">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="I283" t="str">
-        <f>_xlfn.CONCAT(G283,"_",D283)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="284" spans="1:9">
@@ -10721,17 +10721,17 @@
         <v>0</v>
       </c>
       <c r="F284" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G284" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H284" s="22">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I284" t="str">
-        <f>_xlfn.CONCAT(G284,"_",D284)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="285" spans="1:9">
@@ -10751,17 +10751,17 @@
         <v>0</v>
       </c>
       <c r="F285" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G285" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H285" s="22">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I285" t="str">
-        <f>_xlfn.CONCAT(G285,"_",D285)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="286" spans="1:9">
@@ -10781,17 +10781,17 @@
         <v>0</v>
       </c>
       <c r="F286" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G286" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H286" s="22">
-        <v>136</v>
+        <v>169</v>
       </c>
       <c r="I286" t="str">
-        <f>_xlfn.CONCAT(G286,"_",D286)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="287" spans="1:9">
@@ -10811,17 +10811,17 @@
         <v>0</v>
       </c>
       <c r="F287" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G287" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H287" s="22">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I287" t="str">
-        <f>_xlfn.CONCAT(G287,"_",D287)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="288" spans="1:9">
@@ -10841,17 +10841,17 @@
         <v>0</v>
       </c>
       <c r="F288" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G288" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H288" s="22">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="I288" t="str">
-        <f>_xlfn.CONCAT(G288,"_",D288)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="289" spans="1:9">
@@ -10871,17 +10871,17 @@
         <v>0</v>
       </c>
       <c r="F289" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G289" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H289" s="22">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I289" t="str">
-        <f>_xlfn.CONCAT(G289,"_",D289)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="290" spans="1:9">
@@ -10901,17 +10901,17 @@
         <v>0</v>
       </c>
       <c r="F290" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G290" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H290" s="22">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I290" t="str">
-        <f>_xlfn.CONCAT(G290,"_",D290)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="291" spans="1:9">
@@ -10931,17 +10931,17 @@
         <v>0</v>
       </c>
       <c r="F291" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G291" s="22" t="s">
-        <v>248</v>
+        <v>13</v>
       </c>
       <c r="H291" s="22">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="I291" t="str">
-        <f>_xlfn.CONCAT(G291,"_",D291)</f>
-        <v>metadecoder_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_FALSE</v>
       </c>
     </row>
     <row r="292" spans="1:9">
@@ -10955,7 +10955,7 @@
         <v>0</v>
       </c>
       <c r="D292" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E292" s="22" t="b">
         <v>0</v>
@@ -10967,11 +10967,11 @@
         <v>13</v>
       </c>
       <c r="H292" s="22">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="I292" t="str">
-        <f>_xlfn.CONCAT(G292,"_",D292)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="293" spans="1:9">
@@ -10985,7 +10985,7 @@
         <v>0</v>
       </c>
       <c r="D293" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E293" s="22" t="b">
         <v>0</v>
@@ -10997,11 +10997,11 @@
         <v>13</v>
       </c>
       <c r="H293" s="22">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="I293" t="str">
-        <f>_xlfn.CONCAT(G293,"_",D293)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="294" spans="1:9">
@@ -11015,7 +11015,7 @@
         <v>0</v>
       </c>
       <c r="D294" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E294" s="22" t="b">
         <v>0</v>
@@ -11027,11 +11027,11 @@
         <v>13</v>
       </c>
       <c r="H294" s="22">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="I294" t="str">
-        <f>_xlfn.CONCAT(G294,"_",D294)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="295" spans="1:9">
@@ -11045,7 +11045,7 @@
         <v>0</v>
       </c>
       <c r="D295" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E295" s="22" t="b">
         <v>0</v>
@@ -11057,11 +11057,11 @@
         <v>13</v>
       </c>
       <c r="H295" s="22">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="I295" t="str">
-        <f>_xlfn.CONCAT(G295,"_",D295)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="296" spans="1:9">
@@ -11075,7 +11075,7 @@
         <v>0</v>
       </c>
       <c r="D296" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E296" s="22" t="b">
         <v>0</v>
@@ -11087,11 +11087,11 @@
         <v>13</v>
       </c>
       <c r="H296" s="22">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I296" t="str">
-        <f>_xlfn.CONCAT(G296,"_",D296)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="297" spans="1:9">
@@ -11105,7 +11105,7 @@
         <v>0</v>
       </c>
       <c r="D297" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E297" s="22" t="b">
         <v>0</v>
@@ -11117,11 +11117,11 @@
         <v>13</v>
       </c>
       <c r="H297" s="22">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="I297" t="str">
-        <f>_xlfn.CONCAT(G297,"_",D297)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="298" spans="1:9">
@@ -11135,7 +11135,7 @@
         <v>0</v>
       </c>
       <c r="D298" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E298" s="22" t="b">
         <v>0</v>
@@ -11147,11 +11147,11 @@
         <v>13</v>
       </c>
       <c r="H298" s="22">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="I298" t="str">
-        <f>_xlfn.CONCAT(G298,"_",D298)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="299" spans="1:9">
@@ -11165,7 +11165,7 @@
         <v>0</v>
       </c>
       <c r="D299" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E299" s="22" t="b">
         <v>0</v>
@@ -11177,11 +11177,11 @@
         <v>13</v>
       </c>
       <c r="H299" s="22">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="I299" t="str">
-        <f>_xlfn.CONCAT(G299,"_",D299)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="300" spans="1:9">
@@ -11195,7 +11195,7 @@
         <v>0</v>
       </c>
       <c r="D300" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E300" s="22" t="b">
         <v>0</v>
@@ -11207,11 +11207,11 @@
         <v>13</v>
       </c>
       <c r="H300" s="22">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="I300" t="str">
-        <f>_xlfn.CONCAT(G300,"_",D300)</f>
-        <v>AVAMB_FALSE</v>
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
       </c>
     </row>
     <row r="301" spans="1:9">
@@ -11225,7 +11225,7 @@
         <v>0</v>
       </c>
       <c r="D301" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E301" s="22" t="b">
         <v>0</v>
@@ -11237,311 +11237,311 @@
         <v>13</v>
       </c>
       <c r="H301" s="22">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="I301" t="str">
-        <f>_xlfn.CONCAT(G301,"_",D301)</f>
-        <v>AVAMB_FALSE</v>
-      </c>
-    </row>
-    <row r="302" spans="1:9">
-      <c r="A302" s="22" t="s">
+        <f t="shared" si="5"/>
+        <v>AVAMB_TRUE</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" ht="16">
+      <c r="A302" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B302" s="22" t="b">
-        <v>0</v>
+      <c r="B302" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="C302" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D302" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E302" s="22" t="b">
         <v>0</v>
       </c>
       <c r="F302" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G302" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H302" s="22">
-        <v>108</v>
+        <v>235</v>
+      </c>
+      <c r="H302" s="32">
+        <v>145</v>
       </c>
       <c r="I302" t="str">
-        <f>_xlfn.CONCAT(G302,"_",D302)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="303" spans="1:9">
-      <c r="A303" s="22" t="s">
+        <f t="shared" si="5"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" ht="16">
+      <c r="A303" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B303" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C303" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D303" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E303" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F303" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G303" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H303" s="32">
+        <v>206</v>
+      </c>
+      <c r="I303" t="str">
+        <f t="shared" si="5"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" ht="16">
+      <c r="A304" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B304" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C304" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D304" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E304" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F304" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G304" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H304" s="32">
+        <v>158</v>
+      </c>
+      <c r="I304" t="str">
+        <f t="shared" ref="I304:I321" si="6">_xlfn.CONCAT(G304,"_",D304)</f>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" ht="16">
+      <c r="A305" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B305" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C305" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D305" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E305" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F305" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G305" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H305" s="32">
+        <v>180</v>
+      </c>
+      <c r="I305" t="str">
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" ht="16">
+      <c r="A306" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B303" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C303" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D303" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E303" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F303" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G303" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H303" s="22">
-        <v>126</v>
-      </c>
-      <c r="I303" t="str">
-        <f>_xlfn.CONCAT(G303,"_",D303)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9">
-      <c r="A304" s="22" t="s">
+      <c r="B306" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C306" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D306" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E306" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F306" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G306" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H306" s="32">
+        <v>116</v>
+      </c>
+      <c r="I306" t="str">
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" ht="16">
+      <c r="A307" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B307" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C307" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D307" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E307" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F307" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G307" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H307" s="32">
+        <v>100</v>
+      </c>
+      <c r="I307" t="str">
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" ht="16">
+      <c r="A308" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B308" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C308" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D308" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E308" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F308" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G308" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H308" s="32">
+        <v>163</v>
+      </c>
+      <c r="I308" t="str">
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" ht="16">
+      <c r="A309" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B304" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C304" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D304" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E304" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F304" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G304" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H304" s="22">
+      <c r="B309" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C309" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D309" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E309" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F309" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G309" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H309" s="32">
         <v>143</v>
       </c>
-      <c r="I304" t="str">
-        <f>_xlfn.CONCAT(G304,"_",D304)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="305" spans="1:9">
-      <c r="A305" s="22" t="s">
+      <c r="I309" t="str">
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" ht="16">
+      <c r="A310" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B305" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C305" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D305" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E305" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F305" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G305" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H305" s="22">
-        <v>161</v>
-      </c>
-      <c r="I305" t="str">
-        <f>_xlfn.CONCAT(G305,"_",D305)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="306" spans="1:9">
-      <c r="A306" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B306" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C306" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D306" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E306" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F306" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G306" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H306" s="22">
-        <v>179</v>
-      </c>
-      <c r="I306" t="str">
-        <f>_xlfn.CONCAT(G306,"_",D306)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="307" spans="1:9">
-      <c r="A307" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B307" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C307" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D307" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E307" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F307" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G307" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H307" s="22">
-        <v>113</v>
-      </c>
-      <c r="I307" t="str">
-        <f>_xlfn.CONCAT(G307,"_",D307)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="308" spans="1:9">
-      <c r="A308" s="22" t="s">
+      <c r="B310" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C310" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D310" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E310" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F310" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G310" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="H310" s="32">
+        <v>134</v>
+      </c>
+      <c r="I310" t="str">
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" ht="16">
+      <c r="A311" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B308" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C308" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D308" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E308" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F308" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G308" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H308" s="22">
-        <v>127</v>
-      </c>
-      <c r="I308" t="str">
-        <f>_xlfn.CONCAT(G308,"_",D308)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="309" spans="1:9">
-      <c r="A309" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B309" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C309" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D309" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E309" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F309" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G309" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H309" s="22">
-        <v>149</v>
-      </c>
-      <c r="I309" t="str">
-        <f>_xlfn.CONCAT(G309,"_",D309)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="310" spans="1:9">
-      <c r="A310" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B310" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C310" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D310" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E310" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F310" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G310" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H310" s="22">
-        <v>167</v>
-      </c>
-      <c r="I310" t="str">
-        <f>_xlfn.CONCAT(G310,"_",D310)</f>
-        <v>AVAMB_TRUE</v>
-      </c>
-    </row>
-    <row r="311" spans="1:9">
-      <c r="A311" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B311" s="22" t="b">
-        <v>1</v>
+      <c r="B311" s="32" t="b">
+        <v>0</v>
       </c>
       <c r="C311" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D311" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E311" s="22" t="b">
         <v>0</v>
       </c>
       <c r="F311" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G311" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H311" s="22">
-        <v>184</v>
+        <v>235</v>
+      </c>
+      <c r="H311" s="32">
+        <v>107</v>
       </c>
       <c r="I311" t="str">
-        <f>_xlfn.CONCAT(G311,"_",D311)</f>
-        <v>AVAMB_TRUE</v>
+        <f t="shared" si="6"/>
+        <v>comebin_FALSE</v>
       </c>
     </row>
     <row r="312" spans="1:9" ht="16">
@@ -11555,7 +11555,7 @@
         <v>0</v>
       </c>
       <c r="D312" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E312" s="22" t="b">
         <v>0</v>
@@ -11564,14 +11564,14 @@
         <v>0</v>
       </c>
       <c r="G312" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H312" s="32">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="I312" t="str">
-        <f>_xlfn.CONCAT(G312,"_",D312)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="313" spans="1:9" ht="16">
@@ -11585,7 +11585,7 @@
         <v>0</v>
       </c>
       <c r="D313" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E313" s="22" t="b">
         <v>0</v>
@@ -11594,14 +11594,14 @@
         <v>0</v>
       </c>
       <c r="G313" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H313" s="32">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="I313" t="str">
-        <f>_xlfn.CONCAT(G313,"_",D313)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="314" spans="1:9" ht="16">
@@ -11615,7 +11615,7 @@
         <v>0</v>
       </c>
       <c r="D314" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E314" s="22" t="b">
         <v>0</v>
@@ -11624,14 +11624,14 @@
         <v>0</v>
       </c>
       <c r="G314" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H314" s="32">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I314" t="str">
-        <f>_xlfn.CONCAT(G314,"_",D314)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="315" spans="1:9" ht="16">
@@ -11645,7 +11645,7 @@
         <v>0</v>
       </c>
       <c r="D315" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E315" s="22" t="b">
         <v>0</v>
@@ -11654,14 +11654,14 @@
         <v>0</v>
       </c>
       <c r="G315" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H315" s="32">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="I315" t="str">
-        <f>_xlfn.CONCAT(G315,"_",D315)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="316" spans="1:9" ht="16">
@@ -11675,7 +11675,7 @@
         <v>0</v>
       </c>
       <c r="D316" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E316" s="22" t="b">
         <v>0</v>
@@ -11684,14 +11684,14 @@
         <v>0</v>
       </c>
       <c r="G316" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H316" s="32">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="I316" t="str">
-        <f>_xlfn.CONCAT(G316,"_",D316)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="317" spans="1:9" ht="16">
@@ -11705,7 +11705,7 @@
         <v>0</v>
       </c>
       <c r="D317" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E317" s="22" t="b">
         <v>0</v>
@@ -11714,14 +11714,14 @@
         <v>0</v>
       </c>
       <c r="G317" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H317" s="32">
         <v>100</v>
       </c>
       <c r="I317" t="str">
-        <f>_xlfn.CONCAT(G317,"_",D317)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="318" spans="1:9" ht="16">
@@ -11735,7 +11735,7 @@
         <v>0</v>
       </c>
       <c r="D318" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E318" s="22" t="b">
         <v>0</v>
@@ -11744,14 +11744,14 @@
         <v>0</v>
       </c>
       <c r="G318" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H318" s="32">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="I318" t="str">
-        <f>_xlfn.CONCAT(G318,"_",D318)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="319" spans="1:9" ht="16">
@@ -11765,7 +11765,7 @@
         <v>0</v>
       </c>
       <c r="D319" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E319" s="22" t="b">
         <v>0</v>
@@ -11774,14 +11774,14 @@
         <v>0</v>
       </c>
       <c r="G319" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H319" s="32">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="I319" t="str">
-        <f>_xlfn.CONCAT(G319,"_",D319)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="320" spans="1:9" ht="16">
@@ -11795,7 +11795,7 @@
         <v>0</v>
       </c>
       <c r="D320" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E320" s="22" t="b">
         <v>0</v>
@@ -11804,14 +11804,14 @@
         <v>0</v>
       </c>
       <c r="G320" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H320" s="32">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="I320" t="str">
-        <f>_xlfn.CONCAT(G320,"_",D320)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="321" spans="1:9" ht="16">
@@ -11825,7 +11825,7 @@
         <v>0</v>
       </c>
       <c r="D321" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E321" s="22" t="b">
         <v>0</v>
@@ -11834,14 +11834,14 @@
         <v>0</v>
       </c>
       <c r="G321" s="22" t="s">
-        <v>235</v>
+        <v>267</v>
       </c>
       <c r="H321" s="32">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="I321" t="str">
-        <f>_xlfn.CONCAT(G321,"_",D321)</f>
-        <v>comebin_FALSE</v>
+        <f t="shared" si="6"/>
+        <v>semibin_TRUE</v>
       </c>
     </row>
     <row r="322" spans="1:9" ht="16">
@@ -11849,13 +11849,13 @@
         <v>4</v>
       </c>
       <c r="B322" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C322" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D322" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E322" s="22" t="b">
         <v>0</v>
@@ -11864,14 +11864,14 @@
         <v>0</v>
       </c>
       <c r="G322" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H322" s="32">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I322" t="str">
-        <f>_xlfn.CONCAT(G322,"_",D322)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" ref="I322:I341" si="7">_xlfn.CONCAT(G322,"_",D322)</f>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="323" spans="1:9" ht="16">
@@ -11879,13 +11879,13 @@
         <v>9</v>
       </c>
       <c r="B323" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C323" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D323" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E323" s="22" t="b">
         <v>0</v>
@@ -11894,14 +11894,14 @@
         <v>0</v>
       </c>
       <c r="G323" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H323" s="32">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="I323" t="str">
-        <f>_xlfn.CONCAT(G323,"_",D323)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="324" spans="1:9" ht="16">
@@ -11909,13 +11909,13 @@
         <v>7</v>
       </c>
       <c r="B324" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C324" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D324" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E324" s="22" t="b">
         <v>0</v>
@@ -11924,14 +11924,14 @@
         <v>0</v>
       </c>
       <c r="G324" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H324" s="32">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="I324" t="str">
-        <f>_xlfn.CONCAT(G324,"_",D324)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="325" spans="1:9" ht="16">
@@ -11939,13 +11939,13 @@
         <v>8</v>
       </c>
       <c r="B325" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C325" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D325" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E325" s="22" t="b">
         <v>0</v>
@@ -11954,14 +11954,14 @@
         <v>0</v>
       </c>
       <c r="G325" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H325" s="32">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="I325" t="str">
-        <f>_xlfn.CONCAT(G325,"_",D325)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="326" spans="1:9" ht="16">
@@ -11969,13 +11969,13 @@
         <v>6</v>
       </c>
       <c r="B326" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C326" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D326" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E326" s="22" t="b">
         <v>0</v>
@@ -11984,14 +11984,14 @@
         <v>0</v>
       </c>
       <c r="G326" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H326" s="32">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="I326" t="str">
-        <f>_xlfn.CONCAT(G326,"_",D326)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="327" spans="1:9" ht="16">
@@ -11999,13 +11999,13 @@
         <v>4</v>
       </c>
       <c r="B327" s="32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C327" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D327" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E327" s="22" t="b">
         <v>0</v>
@@ -12014,14 +12014,14 @@
         <v>0</v>
       </c>
       <c r="G327" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H327" s="32">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="I327" t="str">
-        <f>_xlfn.CONCAT(G327,"_",D327)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="328" spans="1:9" ht="16">
@@ -12029,13 +12029,13 @@
         <v>9</v>
       </c>
       <c r="B328" s="32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C328" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D328" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E328" s="22" t="b">
         <v>0</v>
@@ -12044,14 +12044,14 @@
         <v>0</v>
       </c>
       <c r="G328" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H328" s="32">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I328" t="str">
-        <f>_xlfn.CONCAT(G328,"_",D328)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="329" spans="1:9" ht="16">
@@ -12059,13 +12059,13 @@
         <v>7</v>
       </c>
       <c r="B329" s="32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C329" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D329" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E329" s="22" t="b">
         <v>0</v>
@@ -12074,14 +12074,14 @@
         <v>0</v>
       </c>
       <c r="G329" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H329" s="32">
         <v>149</v>
       </c>
       <c r="I329" t="str">
-        <f>_xlfn.CONCAT(G329,"_",D329)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="330" spans="1:9" ht="16">
@@ -12089,13 +12089,13 @@
         <v>8</v>
       </c>
       <c r="B330" s="32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C330" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D330" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E330" s="22" t="b">
         <v>0</v>
@@ -12104,14 +12104,14 @@
         <v>0</v>
       </c>
       <c r="G330" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H330" s="32">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I330" t="str">
-        <f>_xlfn.CONCAT(G330,"_",D330)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="331" spans="1:9" ht="16">
@@ -12119,13 +12119,13 @@
         <v>6</v>
       </c>
       <c r="B331" s="32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C331" s="22" t="b">
         <v>0</v>
       </c>
       <c r="D331" s="22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E331" s="22" t="b">
         <v>0</v>
@@ -12134,14 +12134,14 @@
         <v>0</v>
       </c>
       <c r="G331" s="22" t="s">
-        <v>267</v>
+        <v>522</v>
       </c>
       <c r="H331" s="32">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I331" t="str">
-        <f>_xlfn.CONCAT(G331,"_",D331)</f>
-        <v>semibin_TRUE</v>
+        <f t="shared" si="7"/>
+        <v>comebin_single_FALSE</v>
       </c>
     </row>
     <row r="332" spans="1:9" ht="16">
@@ -12164,14 +12164,14 @@
         <v>0</v>
       </c>
       <c r="G332" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H332" s="32">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="I332" t="str">
-        <f t="shared" ref="I332:I341" si="5">_xlfn.CONCAT(G332,"_",D332)</f>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="333" spans="1:9" ht="16">
@@ -12194,14 +12194,14 @@
         <v>0</v>
       </c>
       <c r="G333" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H333" s="32">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="I333" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="334" spans="1:9" ht="16">
@@ -12224,14 +12224,14 @@
         <v>0</v>
       </c>
       <c r="G334" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H334" s="32">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="I334" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="335" spans="1:9" ht="16">
@@ -12254,14 +12254,14 @@
         <v>0</v>
       </c>
       <c r="G335" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H335" s="32">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="I335" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="336" spans="1:9" ht="16">
@@ -12284,14 +12284,14 @@
         <v>0</v>
       </c>
       <c r="G336" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H336" s="32">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="I336" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="337" spans="1:9" ht="16">
@@ -12314,14 +12314,14 @@
         <v>0</v>
       </c>
       <c r="G337" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H337" s="32">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="I337" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="338" spans="1:9" ht="16">
@@ -12344,14 +12344,14 @@
         <v>0</v>
       </c>
       <c r="G338" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H338" s="32">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="I338" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="339" spans="1:9" ht="16">
@@ -12374,14 +12374,14 @@
         <v>0</v>
       </c>
       <c r="G339" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H339" s="32">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="I339" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="340" spans="1:9" ht="16">
@@ -12404,14 +12404,14 @@
         <v>0</v>
       </c>
       <c r="G340" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H340" s="32">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="I340" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
     <row r="341" spans="1:9" ht="16">
@@ -12434,14 +12434,14 @@
         <v>0</v>
       </c>
       <c r="G341" s="22" t="s">
-        <v>522</v>
+        <v>267</v>
       </c>
       <c r="H341" s="32">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="I341" t="str">
-        <f t="shared" si="5"/>
-        <v>comebin_single_FALSE</v>
+        <f t="shared" si="7"/>
+        <v>semibin_FALSE</v>
       </c>
     </row>
   </sheetData>
@@ -14630,7 +14630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD03773-EAA3-B544-A37A-98227B841396}">
   <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+    <sheetView topLeftCell="A149" workbookViewId="0">
       <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>

</xml_diff>